<commit_message>
revise team meeting record
</commit_message>
<xml_diff>
--- a/08_Management/Project_Team_Meeting-BCD1-0117_BCDCarpentryProject.xlsx
+++ b/08_Management/Project_Team_Meeting-BCD1-0117_BCDCarpentryProject.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>3/3/2017</t>
-  </si>
-  <si>
-    <t>10:00AM</t>
   </si>
   <si>
     <t>E202</t>
@@ -52,9 +49,6 @@
     <t>8/3/2017</t>
   </si>
   <si>
-    <t>09:55AM</t>
-  </si>
-  <si>
     <t>Met before client meeting
 Went over questions and eliminated duplicate questions</t>
   </si>
@@ -62,9 +56,6 @@
     <t>10/3/2017</t>
   </si>
   <si>
-    <t>1:55PM</t>
-  </si>
-  <si>
     <t>E204</t>
   </si>
   <si>
@@ -79,9 +70,6 @@
     <t>13/3/2017</t>
   </si>
   <si>
-    <t>09:30AM</t>
-  </si>
-  <si>
     <t>Spoke briefly about what we would discuss with the client at their workplace
 Spoke after meeting with client as to our next steps</t>
   </si>
@@ -89,16 +77,10 @@
     <t>15/3/2017</t>
   </si>
   <si>
-    <t>01:55PM</t>
-  </si>
-  <si>
     <t>Spoke on break in class about progress.</t>
   </si>
   <si>
     <t>27/3/2017</t>
-  </si>
-  <si>
-    <t>9:55AM</t>
   </si>
   <si>
     <t>Tao Sun
@@ -119,9 +101,6 @@
     <t>30/3/2017</t>
   </si>
   <si>
-    <t>12:55PM</t>
-  </si>
-  <si>
     <t>Discussed further progress and future concepts</t>
   </si>
   <si>
@@ -147,17 +126,11 @@
     <t>12/4/2017</t>
   </si>
   <si>
-    <t>11:48AM</t>
-  </si>
-  <si>
     <t>Tao sent an email contained all logical and conceptual diagrams as well as 
 database coding to other group members.</t>
   </si>
   <si>
     <t>1/5/2017</t>
-  </si>
-  <si>
-    <t>11:55AM</t>
   </si>
   <si>
     <t>Discuss what we have done in the study break,
@@ -181,9 +154,6 @@
     <t>4/5/2017</t>
   </si>
   <si>
-    <t>12:55AM</t>
-  </si>
-  <si>
     <t>Discuss second presentation and talk more about progress on front-end application</t>
   </si>
   <si>
@@ -194,13 +164,46 @@
   </si>
   <si>
     <t>Sent meeting minutes to Sunil for review</t>
+  </si>
+  <si>
+    <t>Discuss weekend progress</t>
+  </si>
+  <si>
+    <t>Reallocate tasks due to Damian's inexperience with ASP.net</t>
+  </si>
+  <si>
+    <t>Discuss progress on deliverables so far.
+Have a look over completed program and database.</t>
+  </si>
+  <si>
+    <t>Discuss system installation at BCD Carpentry. 
+Discuss further actions at this point.</t>
+  </si>
+  <si>
+    <t>Discuss upcoming presentations and progress.
+Consider changes requested by client and whether they're feasible at this point.</t>
+  </si>
+  <si>
+    <t>Tao asked us other two to work on poster-related deliverables.</t>
+  </si>
+  <si>
+    <t>Discuss what has been changed and what hasn't in program.
+Discuss future actions regarding presentation and poster creation.</t>
+  </si>
+  <si>
+    <t>Discuss installing final copy of the system on client's computer and oral presentation
+taking place that afternoon.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="177" formatCode="hh:mm"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +231,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,12 +254,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFBD4B4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6DDE8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,8 +275,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBD4B4"/>
+        <bgColor rgb="FFFBD4B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6DDE8"/>
+        <bgColor rgb="FFB6DDE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5B8B7"/>
+        <bgColor rgb="FFE5B8B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6E3BC"/>
+        <bgColor rgb="FFD6E3BC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCC0D9"/>
+        <bgColor rgb="FFCCC0D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -282,62 +315,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -345,40 +333,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -699,293 +685,429 @@
     <col min="5" max="5" width="75.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="B4" s="3">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="B7" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="E10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="E11" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B12" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="2" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="B13" s="3">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="B14" s="3">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="2" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="B15" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="E15" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="16" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B16" s="3">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="B17" s="9">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="D17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>42864</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+    <row r="19" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>42865</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.54861111111111116</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>42871</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="2" t="s">
+    </row>
+    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>42872</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+    <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>42880</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="9" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>42883</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2" t="s">
+    </row>
+    <row r="24" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>42885</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+    <row r="25" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>42887</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" s="11">
-        <v>0.4548611111111111</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>